<commit_message>
modified:   data.csv 	modified:   data.xlsx 	modified:   getcuaca.js 	new file:   getcuaca2.js 	modified:   package.json
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -618,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="H7" t="str">
-        <v/>
-      </c>
-      <c r="I7" t="str">
-        <v/>
+        <v>s 10:57</v>
+      </c>
+      <c r="I7">
+        <v>29</v>
       </c>
       <c r="J7" t="str">
-        <v/>
+        <v>cerah</v>
       </c>
     </row>
     <row r="8">
@@ -632,22 +632,22 @@
         <v>Jumat 26/09/2025 12:00</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" t="str">
-        <v>Cerah Berawan</v>
+        <v>Cerah</v>
       </c>
       <c r="E8" t="str">
-        <v>E (118°)</v>
+        <v>E (115°)</v>
       </c>
       <c r="F8">
-        <v>15.8</v>
+        <v>12.2</v>
       </c>
       <c r="G8">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H8" t="str">
         <v/>
@@ -734,16 +734,16 @@
         <v>69</v>
       </c>
       <c r="D11" t="str">
-        <v>Hujan Ringan</v>
+        <v>Berawan</v>
       </c>
       <c r="E11" t="str">
-        <v>E (113°)</v>
+        <v>E (114°)</v>
       </c>
       <c r="F11">
-        <v>14.7</v>
+        <v>12.9</v>
       </c>
       <c r="G11">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H11" t="str">
         <v/>
@@ -827,19 +827,19 @@
         <v>27</v>
       </c>
       <c r="C14">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D14" t="str">
         <v>Berawan</v>
       </c>
       <c r="E14" t="str">
-        <v>E (125°)</v>
+        <v>E (102°)</v>
       </c>
       <c r="F14">
-        <v>12</v>
+        <v>9.9</v>
       </c>
       <c r="G14">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H14" t="str">
         <v/>
@@ -923,19 +923,19 @@
         <v>29</v>
       </c>
       <c r="C17">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D17" t="str">
-        <v>Cerah</v>
+        <v>Berawan</v>
       </c>
       <c r="E17" t="str">
-        <v>NE (81°)</v>
+        <v>E (100°)</v>
       </c>
       <c r="F17">
-        <v>12</v>
+        <v>17.2</v>
       </c>
       <c r="G17">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H17" t="str">
         <v/>
@@ -1019,19 +1019,19 @@
         <v>31</v>
       </c>
       <c r="C20">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D20" t="str">
-        <v>Cerah Berawan</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E20" t="str">
-        <v>E (122°)</v>
+        <v>SE (170°)</v>
       </c>
       <c r="F20">
-        <v>14.3</v>
+        <v>18.5</v>
       </c>
       <c r="G20">
-        <v>0.2</v>
+        <v>1.3</v>
       </c>
       <c r="H20" t="str">
         <v/>
@@ -1112,22 +1112,22 @@
         <v>Sabtu 27/09/2025 15:00</v>
       </c>
       <c r="B23">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" t="str">
-        <v>Cerah Berawan</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E23" t="str">
-        <v>E (122°)</v>
+        <v>E (120°)</v>
       </c>
       <c r="F23">
-        <v>14.3</v>
+        <v>9.4</v>
       </c>
       <c r="G23">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="H23" t="str">
         <v/>
@@ -1217,13 +1217,13 @@
         <v>Cerah Berawan</v>
       </c>
       <c r="E26" t="str">
-        <v>NE (88°)</v>
+        <v>E (120°)</v>
       </c>
       <c r="F26">
-        <v>8.7</v>
+        <v>9.2</v>
       </c>
       <c r="G26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H26" t="str">
         <v/>
@@ -1291,11 +1291,23 @@
       <c r="A29" t="str">
         <v>Minggu 28/09/2025 09:00</v>
       </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>72</v>
+      </c>
       <c r="D29" t="str">
-        <v>Tidak ada data</v>
+        <v>Cerah Berawan</v>
       </c>
       <c r="E29" t="str">
-        <v/>
+        <v>N (40°)</v>
+      </c>
+      <c r="F29">
+        <v>10.5</v>
+      </c>
+      <c r="G29">
+        <v>0.7</v>
       </c>
       <c r="H29" t="str">
         <v/>
@@ -1357,11 +1369,23 @@
       <c r="A32" t="str">
         <v>Minggu 28/09/2025 12:00</v>
       </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>66</v>
+      </c>
       <c r="D32" t="str">
-        <v>Tidak ada data</v>
+        <v>Berawan</v>
       </c>
       <c r="E32" t="str">
-        <v/>
+        <v>E (112°)</v>
+      </c>
+      <c r="F32">
+        <v>16.7</v>
+      </c>
+      <c r="G32">
+        <v>0.7</v>
       </c>
       <c r="H32" t="str">
         <v/>
@@ -1423,11 +1447,23 @@
       <c r="A35" t="str">
         <v>Minggu 28/09/2025 15:00</v>
       </c>
+      <c r="B35">
+        <v>30</v>
+      </c>
+      <c r="C35">
+        <v>71</v>
+      </c>
       <c r="D35" t="str">
-        <v>Tidak ada data</v>
+        <v>Berawan</v>
       </c>
       <c r="E35" t="str">
-        <v/>
+        <v>E (112°)</v>
+      </c>
+      <c r="F35">
+        <v>16.7</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
       </c>
       <c r="H35" t="str">
         <v/>
@@ -1489,11 +1525,23 @@
       <c r="A38" t="str">
         <v>Minggu 28/09/2025 18:00</v>
       </c>
+      <c r="B38">
+        <v>27</v>
+      </c>
+      <c r="C38">
+        <v>82</v>
+      </c>
       <c r="D38" t="str">
-        <v>Tidak ada data</v>
+        <v>Berawan</v>
       </c>
       <c r="E38" t="str">
-        <v/>
+        <v>E (103°)</v>
+      </c>
+      <c r="F38">
+        <v>13</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
       </c>
       <c r="H38" t="str">
         <v/>

</xml_diff>

<commit_message>
new api for getcuaca.js
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3153,7 +3153,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J158"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -4170,14 +4170,2809 @@
         <v/>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Selasa 30/09/2025 07:00</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E39" t="str">
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <v/>
+      </c>
+      <c r="J39" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Selasa 30/09/2025 08:00</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E40" t="str">
+        <v/>
+      </c>
+      <c r="H40" t="str">
+        <v/>
+      </c>
+      <c r="I40" t="str">
+        <v/>
+      </c>
+      <c r="J40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Selasa 30/09/2025 09:00</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E41" t="str">
+        <v/>
+      </c>
+      <c r="H41" t="str">
+        <v/>
+      </c>
+      <c r="I41" t="str">
+        <v/>
+      </c>
+      <c r="J41" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Selasa 30/09/2025 10:00</v>
+      </c>
+      <c r="B42">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>75</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E42" t="str">
+        <v>NW (347°)</v>
+      </c>
+      <c r="F42">
+        <v>5.2</v>
+      </c>
+      <c r="G42">
+        <v>1.7</v>
+      </c>
+      <c r="H42" t="str">
+        <v/>
+      </c>
+      <c r="I42" t="str">
+        <v/>
+      </c>
+      <c r="J42" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Selasa 30/09/2025 11:00</v>
+      </c>
+      <c r="B43">
+        <v>29</v>
+      </c>
+      <c r="C43">
+        <v>72</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E43" t="str">
+        <v>NW (347°)</v>
+      </c>
+      <c r="F43">
+        <v>5.2</v>
+      </c>
+      <c r="G43">
+        <v>2.7</v>
+      </c>
+      <c r="H43" t="str">
+        <v/>
+      </c>
+      <c r="I43" t="str">
+        <v/>
+      </c>
+      <c r="J43" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Selasa 30/09/2025 12:00</v>
+      </c>
+      <c r="B44">
+        <v>30</v>
+      </c>
+      <c r="C44">
+        <v>69</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E44" t="str">
+        <v>E (114°)</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>2.7</v>
+      </c>
+      <c r="H44" t="str">
+        <v/>
+      </c>
+      <c r="I44" t="str">
+        <v/>
+      </c>
+      <c r="J44" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Selasa 30/09/2025 13:00</v>
+      </c>
+      <c r="B45">
+        <v>31</v>
+      </c>
+      <c r="C45">
+        <v>67</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E45" t="str">
+        <v>E (114°)</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>2.7</v>
+      </c>
+      <c r="H45" t="str">
+        <v/>
+      </c>
+      <c r="I45" t="str">
+        <v/>
+      </c>
+      <c r="J45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Selasa 30/09/2025 14:00</v>
+      </c>
+      <c r="B46">
+        <v>29</v>
+      </c>
+      <c r="C46">
+        <v>78</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E46" t="str">
+        <v>E (114°)</v>
+      </c>
+      <c r="F46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>2.7</v>
+      </c>
+      <c r="H46" t="str">
+        <v/>
+      </c>
+      <c r="I46" t="str">
+        <v/>
+      </c>
+      <c r="J46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Selasa 30/09/2025 15:00</v>
+      </c>
+      <c r="B47">
+        <v>26</v>
+      </c>
+      <c r="C47">
+        <v>90</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E47" t="str">
+        <v>NE (62°)</v>
+      </c>
+      <c r="F47">
+        <v>5.3</v>
+      </c>
+      <c r="G47">
+        <v>2.7</v>
+      </c>
+      <c r="H47" t="str">
+        <v/>
+      </c>
+      <c r="I47" t="str">
+        <v/>
+      </c>
+      <c r="J47" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Selasa 30/09/2025 16:00</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <v>91</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E48" t="str">
+        <v>NE (62°)</v>
+      </c>
+      <c r="F48">
+        <v>5.3</v>
+      </c>
+      <c r="G48">
+        <v>2.7</v>
+      </c>
+      <c r="H48" t="str">
+        <v/>
+      </c>
+      <c r="I48" t="str">
+        <v/>
+      </c>
+      <c r="J48" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Selasa 30/09/2025 17:00</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>93</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E49" t="str">
+        <v>NE (62°)</v>
+      </c>
+      <c r="F49">
+        <v>5.3</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49" t="str">
+        <v/>
+      </c>
+      <c r="I49" t="str">
+        <v/>
+      </c>
+      <c r="J49" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Selasa 30/09/2025 18:00</v>
+      </c>
+      <c r="B50">
+        <v>24</v>
+      </c>
+      <c r="C50">
+        <v>96</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E50" t="str">
+        <v>N (14°)</v>
+      </c>
+      <c r="F50">
+        <v>4.2</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50" t="str">
+        <v/>
+      </c>
+      <c r="I50" t="str">
+        <v/>
+      </c>
+      <c r="J50" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Rabu 01/10/2025 07:00</v>
+      </c>
+      <c r="B51">
+        <v>24</v>
+      </c>
+      <c r="C51">
+        <v>89</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E51" t="str">
+        <v>N (10°)</v>
+      </c>
+      <c r="F51">
+        <v>7.5</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" t="str">
+        <v/>
+      </c>
+      <c r="I51" t="str">
+        <v/>
+      </c>
+      <c r="J51" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Rabu 01/10/2025 08:00</v>
+      </c>
+      <c r="B52">
+        <v>27</v>
+      </c>
+      <c r="C52">
+        <v>81</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E52" t="str">
+        <v>N (10°)</v>
+      </c>
+      <c r="F52">
+        <v>7.5</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" t="str">
+        <v/>
+      </c>
+      <c r="I52" t="str">
+        <v/>
+      </c>
+      <c r="J52" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Rabu 01/10/2025 09:00</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E53" t="str">
+        <v/>
+      </c>
+      <c r="H53" t="str">
+        <v/>
+      </c>
+      <c r="I53" t="str">
+        <v/>
+      </c>
+      <c r="J53" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Rabu 01/10/2025 10:00</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E54" t="str">
+        <v/>
+      </c>
+      <c r="H54" t="str">
+        <v/>
+      </c>
+      <c r="I54" t="str">
+        <v/>
+      </c>
+      <c r="J54" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Rabu 01/10/2025 11:00</v>
+      </c>
+      <c r="B55">
+        <v>31</v>
+      </c>
+      <c r="C55">
+        <v>66</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E55" t="str">
+        <v>NE (70°)</v>
+      </c>
+      <c r="F55">
+        <v>10.5</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55" t="str">
+        <v/>
+      </c>
+      <c r="I55" t="str">
+        <v/>
+      </c>
+      <c r="J55" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Rabu 01/10/2025 12:00</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E56" t="str">
+        <v/>
+      </c>
+      <c r="H56" t="str">
+        <v/>
+      </c>
+      <c r="I56" t="str">
+        <v/>
+      </c>
+      <c r="J56" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Rabu 01/10/2025 13:00</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E57" t="str">
+        <v/>
+      </c>
+      <c r="H57" t="str">
+        <v/>
+      </c>
+      <c r="I57" t="str">
+        <v/>
+      </c>
+      <c r="J57" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Rabu 01/10/2025 14:00</v>
+      </c>
+      <c r="B58">
+        <v>32</v>
+      </c>
+      <c r="C58">
+        <v>64</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Hujan Ringan</v>
+      </c>
+      <c r="E58" t="str">
+        <v>SE (160°)</v>
+      </c>
+      <c r="F58">
+        <v>18.5</v>
+      </c>
+      <c r="G58">
+        <v>1.3</v>
+      </c>
+      <c r="H58" t="str">
+        <v/>
+      </c>
+      <c r="I58" t="str">
+        <v/>
+      </c>
+      <c r="J58" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Rabu 01/10/2025 15:00</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E59" t="str">
+        <v/>
+      </c>
+      <c r="H59" t="str">
+        <v/>
+      </c>
+      <c r="I59" t="str">
+        <v/>
+      </c>
+      <c r="J59" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Rabu 01/10/2025 16:00</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E60" t="str">
+        <v/>
+      </c>
+      <c r="H60" t="str">
+        <v/>
+      </c>
+      <c r="I60" t="str">
+        <v/>
+      </c>
+      <c r="J60" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Rabu 01/10/2025 17:00</v>
+      </c>
+      <c r="B61">
+        <v>30</v>
+      </c>
+      <c r="C61">
+        <v>79</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E61" t="str">
+        <v>S (200°)</v>
+      </c>
+      <c r="F61">
+        <v>18.5</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61" t="str">
+        <v/>
+      </c>
+      <c r="I61" t="str">
+        <v/>
+      </c>
+      <c r="J61" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Rabu 01/10/2025 18:00</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E62" t="str">
+        <v/>
+      </c>
+      <c r="H62" t="str">
+        <v/>
+      </c>
+      <c r="I62" t="str">
+        <v/>
+      </c>
+      <c r="J62" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Kamis 02/10/2025 07:00</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E63" t="str">
+        <v/>
+      </c>
+      <c r="H63" t="str">
+        <v/>
+      </c>
+      <c r="I63" t="str">
+        <v/>
+      </c>
+      <c r="J63" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Kamis 02/10/2025 08:00</v>
+      </c>
+      <c r="B64">
+        <v>27</v>
+      </c>
+      <c r="C64">
+        <v>74</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E64" t="str">
+        <v>N (20°)</v>
+      </c>
+      <c r="F64">
+        <v>8.3</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64" t="str">
+        <v/>
+      </c>
+      <c r="I64" t="str">
+        <v/>
+      </c>
+      <c r="J64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Kamis 02/10/2025 09:00</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E65" t="str">
+        <v/>
+      </c>
+      <c r="H65" t="str">
+        <v/>
+      </c>
+      <c r="I65" t="str">
+        <v/>
+      </c>
+      <c r="J65" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Kamis 02/10/2025 10:00</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E66" t="str">
+        <v/>
+      </c>
+      <c r="H66" t="str">
+        <v/>
+      </c>
+      <c r="I66" t="str">
+        <v/>
+      </c>
+      <c r="J66" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Kamis 02/10/2025 11:00</v>
+      </c>
+      <c r="B67">
+        <v>30</v>
+      </c>
+      <c r="C67">
+        <v>63</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E67" t="str">
+        <v>SE (138°)</v>
+      </c>
+      <c r="F67">
+        <v>13.6</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67" t="str">
+        <v/>
+      </c>
+      <c r="I67" t="str">
+        <v/>
+      </c>
+      <c r="J67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Kamis 02/10/2025 12:00</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E68" t="str">
+        <v/>
+      </c>
+      <c r="H68" t="str">
+        <v/>
+      </c>
+      <c r="I68" t="str">
+        <v/>
+      </c>
+      <c r="J68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Kamis 02/10/2025 13:00</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E69" t="str">
+        <v/>
+      </c>
+      <c r="H69" t="str">
+        <v/>
+      </c>
+      <c r="I69" t="str">
+        <v/>
+      </c>
+      <c r="J69" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Kamis 02/10/2025 14:00</v>
+      </c>
+      <c r="B70">
+        <v>30</v>
+      </c>
+      <c r="C70">
+        <v>65</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E70" t="str">
+        <v>SE (138°)</v>
+      </c>
+      <c r="F70">
+        <v>13.6</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70" t="str">
+        <v/>
+      </c>
+      <c r="I70" t="str">
+        <v/>
+      </c>
+      <c r="J70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Kamis 02/10/2025 15:00</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E71" t="str">
+        <v/>
+      </c>
+      <c r="H71" t="str">
+        <v/>
+      </c>
+      <c r="I71" t="str">
+        <v/>
+      </c>
+      <c r="J71" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Kamis 02/10/2025 16:00</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E72" t="str">
+        <v/>
+      </c>
+      <c r="H72" t="str">
+        <v/>
+      </c>
+      <c r="I72" t="str">
+        <v/>
+      </c>
+      <c r="J72" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Kamis 02/10/2025 17:00</v>
+      </c>
+      <c r="B73">
+        <v>28</v>
+      </c>
+      <c r="C73">
+        <v>77</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E73" t="str">
+        <v>E (127°)</v>
+      </c>
+      <c r="F73">
+        <v>10.8</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73" t="str">
+        <v/>
+      </c>
+      <c r="I73" t="str">
+        <v/>
+      </c>
+      <c r="J73" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Kamis 02/10/2025 18:00</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E74" t="str">
+        <v/>
+      </c>
+      <c r="H74" t="str">
+        <v/>
+      </c>
+      <c r="I74" t="str">
+        <v/>
+      </c>
+      <c r="J74" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Jumat 03/10/2025 07:00</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E75" t="str">
+        <v/>
+      </c>
+      <c r="H75" t="str">
+        <v/>
+      </c>
+      <c r="I75" t="str">
+        <v/>
+      </c>
+      <c r="J75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Jumat 03/10/2025 08:00</v>
+      </c>
+      <c r="B76">
+        <v>29</v>
+      </c>
+      <c r="C76">
+        <v>71</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E76" t="str">
+        <v>E (103°)</v>
+      </c>
+      <c r="F76">
+        <v>5.9</v>
+      </c>
+      <c r="G76">
+        <v>0.2</v>
+      </c>
+      <c r="H76" t="str">
+        <v/>
+      </c>
+      <c r="I76" t="str">
+        <v/>
+      </c>
+      <c r="J76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Jumat 03/10/2025 09:00</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E77" t="str">
+        <v/>
+      </c>
+      <c r="H77" t="str">
+        <v/>
+      </c>
+      <c r="I77" t="str">
+        <v/>
+      </c>
+      <c r="J77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Jumat 03/10/2025 10:00</v>
+      </c>
+      <c r="D78" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E78" t="str">
+        <v/>
+      </c>
+      <c r="H78" t="str">
+        <v/>
+      </c>
+      <c r="I78" t="str">
+        <v/>
+      </c>
+      <c r="J78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Jumat 03/10/2025 11:00</v>
+      </c>
+      <c r="B79">
+        <v>31</v>
+      </c>
+      <c r="C79">
+        <v>64</v>
+      </c>
+      <c r="D79" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E79" t="str">
+        <v>E (131°)</v>
+      </c>
+      <c r="F79">
+        <v>12.3</v>
+      </c>
+      <c r="G79">
+        <v>0.2</v>
+      </c>
+      <c r="H79" t="str">
+        <v/>
+      </c>
+      <c r="I79" t="str">
+        <v/>
+      </c>
+      <c r="J79" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Jumat 03/10/2025 12:00</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E80" t="str">
+        <v/>
+      </c>
+      <c r="H80" t="str">
+        <v/>
+      </c>
+      <c r="I80" t="str">
+        <v/>
+      </c>
+      <c r="J80" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Jumat 03/10/2025 13:00</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E81" t="str">
+        <v/>
+      </c>
+      <c r="H81" t="str">
+        <v/>
+      </c>
+      <c r="I81" t="str">
+        <v/>
+      </c>
+      <c r="J81" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Jumat 03/10/2025 14:00</v>
+      </c>
+      <c r="B82">
+        <v>30</v>
+      </c>
+      <c r="C82">
+        <v>64</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E82" t="str">
+        <v>E (131°)</v>
+      </c>
+      <c r="F82">
+        <v>12.3</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82" t="str">
+        <v/>
+      </c>
+      <c r="I82" t="str">
+        <v/>
+      </c>
+      <c r="J82" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Jumat 03/10/2025 15:00</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E83" t="str">
+        <v/>
+      </c>
+      <c r="H83" t="str">
+        <v/>
+      </c>
+      <c r="I83" t="str">
+        <v/>
+      </c>
+      <c r="J83" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Jumat 03/10/2025 16:00</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E84" t="str">
+        <v/>
+      </c>
+      <c r="H84" t="str">
+        <v/>
+      </c>
+      <c r="I84" t="str">
+        <v/>
+      </c>
+      <c r="J84" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Jumat 03/10/2025 17:00</v>
+      </c>
+      <c r="B85">
+        <v>29</v>
+      </c>
+      <c r="C85">
+        <v>69</v>
+      </c>
+      <c r="D85" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E85" t="str">
+        <v>NE (86°)</v>
+      </c>
+      <c r="F85">
+        <v>14</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85" t="str">
+        <v/>
+      </c>
+      <c r="I85" t="str">
+        <v/>
+      </c>
+      <c r="J85" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Jumat 03/10/2025 18:00</v>
+      </c>
+      <c r="D86" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E86" t="str">
+        <v/>
+      </c>
+      <c r="H86" t="str">
+        <v/>
+      </c>
+      <c r="I86" t="str">
+        <v/>
+      </c>
+      <c r="J86" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Sabtu 04/10/2025 07:00</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E87" t="str">
+        <v/>
+      </c>
+      <c r="H87" t="str">
+        <v/>
+      </c>
+      <c r="I87" t="str">
+        <v/>
+      </c>
+      <c r="J87" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Sabtu 04/10/2025 08:00</v>
+      </c>
+      <c r="B88">
+        <v>27</v>
+      </c>
+      <c r="C88">
+        <v>83</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Cerah Berawan</v>
+      </c>
+      <c r="E88" t="str">
+        <v>NE (81°)</v>
+      </c>
+      <c r="F88">
+        <v>15</v>
+      </c>
+      <c r="G88">
+        <v>0.2</v>
+      </c>
+      <c r="H88" t="str">
+        <v/>
+      </c>
+      <c r="I88" t="str">
+        <v/>
+      </c>
+      <c r="J88" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Sabtu 04/10/2025 09:00</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E89" t="str">
+        <v/>
+      </c>
+      <c r="H89" t="str">
+        <v/>
+      </c>
+      <c r="I89" t="str">
+        <v/>
+      </c>
+      <c r="J89" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Sabtu 04/10/2025 10:00</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E90" t="str">
+        <v/>
+      </c>
+      <c r="H90" t="str">
+        <v/>
+      </c>
+      <c r="I90" t="str">
+        <v/>
+      </c>
+      <c r="J90" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Sabtu 04/10/2025 11:00</v>
+      </c>
+      <c r="D91" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E91" t="str">
+        <v/>
+      </c>
+      <c r="H91" t="str">
+        <v/>
+      </c>
+      <c r="I91" t="str">
+        <v/>
+      </c>
+      <c r="J91" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Sabtu 04/10/2025 12:00</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E92" t="str">
+        <v/>
+      </c>
+      <c r="H92" t="str">
+        <v/>
+      </c>
+      <c r="I92" t="str">
+        <v/>
+      </c>
+      <c r="J92" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Sabtu 04/10/2025 13:00</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E93" t="str">
+        <v/>
+      </c>
+      <c r="H93" t="str">
+        <v/>
+      </c>
+      <c r="I93" t="str">
+        <v/>
+      </c>
+      <c r="J93" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Sabtu 04/10/2025 14:00</v>
+      </c>
+      <c r="B94">
+        <v>29</v>
+      </c>
+      <c r="C94">
+        <v>72</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E94" t="str">
+        <v>E (104°)</v>
+      </c>
+      <c r="F94">
+        <v>7.2</v>
+      </c>
+      <c r="G94">
+        <v>0.2</v>
+      </c>
+      <c r="H94" t="str">
+        <v/>
+      </c>
+      <c r="I94" t="str">
+        <v/>
+      </c>
+      <c r="J94" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>Sabtu 04/10/2025 15:00</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E95" t="str">
+        <v/>
+      </c>
+      <c r="H95" t="str">
+        <v/>
+      </c>
+      <c r="I95" t="str">
+        <v/>
+      </c>
+      <c r="J95" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>Sabtu 04/10/2025 16:00</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E96" t="str">
+        <v/>
+      </c>
+      <c r="H96" t="str">
+        <v/>
+      </c>
+      <c r="I96" t="str">
+        <v/>
+      </c>
+      <c r="J96" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>Sabtu 04/10/2025 17:00</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E97" t="str">
+        <v/>
+      </c>
+      <c r="H97" t="str">
+        <v/>
+      </c>
+      <c r="I97" t="str">
+        <v/>
+      </c>
+      <c r="J97" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>Sabtu 04/10/2025 18:00</v>
+      </c>
+      <c r="D98" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E98" t="str">
+        <v/>
+      </c>
+      <c r="H98" t="str">
+        <v/>
+      </c>
+      <c r="I98" t="str">
+        <v/>
+      </c>
+      <c r="J98" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>Minggu 05/10/2025 07:00</v>
+      </c>
+      <c r="D99" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E99" t="str">
+        <v/>
+      </c>
+      <c r="H99" t="str">
+        <v/>
+      </c>
+      <c r="I99" t="str">
+        <v/>
+      </c>
+      <c r="J99" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>Minggu 05/10/2025 08:00</v>
+      </c>
+      <c r="B100">
+        <v>24</v>
+      </c>
+      <c r="C100">
+        <v>95</v>
+      </c>
+      <c r="D100" t="str">
+        <v>Petir</v>
+      </c>
+      <c r="E100" t="str">
+        <v>N (10°)</v>
+      </c>
+      <c r="F100">
+        <v>1.1</v>
+      </c>
+      <c r="G100">
+        <v>0.3</v>
+      </c>
+      <c r="H100" t="str">
+        <v/>
+      </c>
+      <c r="I100" t="str">
+        <v/>
+      </c>
+      <c r="J100" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>Minggu 05/10/2025 09:00</v>
+      </c>
+      <c r="D101" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E101" t="str">
+        <v/>
+      </c>
+      <c r="H101" t="str">
+        <v/>
+      </c>
+      <c r="I101" t="str">
+        <v/>
+      </c>
+      <c r="J101" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>Minggu 05/10/2025 10:00</v>
+      </c>
+      <c r="D102" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E102" t="str">
+        <v/>
+      </c>
+      <c r="H102" t="str">
+        <v/>
+      </c>
+      <c r="I102" t="str">
+        <v/>
+      </c>
+      <c r="J102" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>Minggu 05/10/2025 11:00</v>
+      </c>
+      <c r="D103" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E103" t="str">
+        <v/>
+      </c>
+      <c r="H103" t="str">
+        <v/>
+      </c>
+      <c r="I103" t="str">
+        <v/>
+      </c>
+      <c r="J103" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>Minggu 05/10/2025 12:00</v>
+      </c>
+      <c r="D104" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E104" t="str">
+        <v/>
+      </c>
+      <c r="H104" t="str">
+        <v/>
+      </c>
+      <c r="I104" t="str">
+        <v/>
+      </c>
+      <c r="J104" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>Minggu 05/10/2025 13:00</v>
+      </c>
+      <c r="D105" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E105" t="str">
+        <v/>
+      </c>
+      <c r="H105" t="str">
+        <v/>
+      </c>
+      <c r="I105" t="str">
+        <v/>
+      </c>
+      <c r="J105" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>Minggu 05/10/2025 14:00</v>
+      </c>
+      <c r="B106">
+        <v>29</v>
+      </c>
+      <c r="C106">
+        <v>72</v>
+      </c>
+      <c r="D106" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E106" t="str">
+        <v>E (99°)</v>
+      </c>
+      <c r="F106">
+        <v>9.5</v>
+      </c>
+      <c r="G106">
+        <v>0.3</v>
+      </c>
+      <c r="H106" t="str">
+        <v/>
+      </c>
+      <c r="I106" t="str">
+        <v/>
+      </c>
+      <c r="J106" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>Minggu 05/10/2025 15:00</v>
+      </c>
+      <c r="D107" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E107" t="str">
+        <v/>
+      </c>
+      <c r="H107" t="str">
+        <v/>
+      </c>
+      <c r="I107" t="str">
+        <v/>
+      </c>
+      <c r="J107" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>Minggu 05/10/2025 16:00</v>
+      </c>
+      <c r="D108" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E108" t="str">
+        <v/>
+      </c>
+      <c r="H108" t="str">
+        <v/>
+      </c>
+      <c r="I108" t="str">
+        <v/>
+      </c>
+      <c r="J108" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>Minggu 05/10/2025 17:00</v>
+      </c>
+      <c r="D109" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E109" t="str">
+        <v/>
+      </c>
+      <c r="H109" t="str">
+        <v/>
+      </c>
+      <c r="I109" t="str">
+        <v/>
+      </c>
+      <c r="J109" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>Minggu 05/10/2025 18:00</v>
+      </c>
+      <c r="D110" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E110" t="str">
+        <v/>
+      </c>
+      <c r="H110" t="str">
+        <v/>
+      </c>
+      <c r="I110" t="str">
+        <v/>
+      </c>
+      <c r="J110" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>Senin 06/10/2025 07:00</v>
+      </c>
+      <c r="D111" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E111" t="str">
+        <v/>
+      </c>
+      <c r="H111" t="str">
+        <v/>
+      </c>
+      <c r="I111" t="str">
+        <v/>
+      </c>
+      <c r="J111" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>Senin 06/10/2025 08:00</v>
+      </c>
+      <c r="B112">
+        <v>23</v>
+      </c>
+      <c r="C112">
+        <v>95</v>
+      </c>
+      <c r="D112" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E112" t="str">
+        <v>SW (246°)</v>
+      </c>
+      <c r="F112">
+        <v>2.6</v>
+      </c>
+      <c r="G112">
+        <v>0.1</v>
+      </c>
+      <c r="H112" t="str">
+        <v/>
+      </c>
+      <c r="I112" t="str">
+        <v/>
+      </c>
+      <c r="J112" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>Senin 06/10/2025 09:00</v>
+      </c>
+      <c r="D113" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E113" t="str">
+        <v/>
+      </c>
+      <c r="H113" t="str">
+        <v/>
+      </c>
+      <c r="I113" t="str">
+        <v/>
+      </c>
+      <c r="J113" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>Senin 06/10/2025 10:00</v>
+      </c>
+      <c r="D114" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E114" t="str">
+        <v/>
+      </c>
+      <c r="H114" t="str">
+        <v/>
+      </c>
+      <c r="I114" t="str">
+        <v/>
+      </c>
+      <c r="J114" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>Senin 06/10/2025 11:00</v>
+      </c>
+      <c r="D115" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E115" t="str">
+        <v/>
+      </c>
+      <c r="H115" t="str">
+        <v/>
+      </c>
+      <c r="I115" t="str">
+        <v/>
+      </c>
+      <c r="J115" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>Senin 06/10/2025 12:00</v>
+      </c>
+      <c r="D116" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E116" t="str">
+        <v/>
+      </c>
+      <c r="H116" t="str">
+        <v/>
+      </c>
+      <c r="I116" t="str">
+        <v/>
+      </c>
+      <c r="J116" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>Senin 06/10/2025 13:00</v>
+      </c>
+      <c r="D117" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E117" t="str">
+        <v/>
+      </c>
+      <c r="H117" t="str">
+        <v/>
+      </c>
+      <c r="I117" t="str">
+        <v/>
+      </c>
+      <c r="J117" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>Senin 06/10/2025 14:00</v>
+      </c>
+      <c r="B118">
+        <v>30</v>
+      </c>
+      <c r="C118">
+        <v>70</v>
+      </c>
+      <c r="D118" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E118" t="str">
+        <v>E (90°)</v>
+      </c>
+      <c r="F118">
+        <v>9.6</v>
+      </c>
+      <c r="G118">
+        <v>0.1</v>
+      </c>
+      <c r="H118" t="str">
+        <v/>
+      </c>
+      <c r="I118" t="str">
+        <v/>
+      </c>
+      <c r="J118" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>Senin 06/10/2025 15:00</v>
+      </c>
+      <c r="D119" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E119" t="str">
+        <v/>
+      </c>
+      <c r="H119" t="str">
+        <v/>
+      </c>
+      <c r="I119" t="str">
+        <v/>
+      </c>
+      <c r="J119" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>Senin 06/10/2025 16:00</v>
+      </c>
+      <c r="D120" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E120" t="str">
+        <v/>
+      </c>
+      <c r="H120" t="str">
+        <v/>
+      </c>
+      <c r="I120" t="str">
+        <v/>
+      </c>
+      <c r="J120" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>Senin 06/10/2025 17:00</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E121" t="str">
+        <v/>
+      </c>
+      <c r="H121" t="str">
+        <v/>
+      </c>
+      <c r="I121" t="str">
+        <v/>
+      </c>
+      <c r="J121" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>Senin 06/10/2025 18:00</v>
+      </c>
+      <c r="D122" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E122" t="str">
+        <v/>
+      </c>
+      <c r="H122" t="str">
+        <v/>
+      </c>
+      <c r="I122" t="str">
+        <v/>
+      </c>
+      <c r="J122" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>Selasa 07/10/2025 07:00</v>
+      </c>
+      <c r="D123" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E123" t="str">
+        <v/>
+      </c>
+      <c r="H123" t="str">
+        <v/>
+      </c>
+      <c r="I123" t="str">
+        <v/>
+      </c>
+      <c r="J123" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>Selasa 07/10/2025 08:00</v>
+      </c>
+      <c r="B124">
+        <v>26</v>
+      </c>
+      <c r="C124">
+        <v>87</v>
+      </c>
+      <c r="D124" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E124" t="str">
+        <v>NE (83°)</v>
+      </c>
+      <c r="F124">
+        <v>6.9</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124" t="str">
+        <v/>
+      </c>
+      <c r="I124" t="str">
+        <v/>
+      </c>
+      <c r="J124" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>Selasa 07/10/2025 09:00</v>
+      </c>
+      <c r="D125" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E125" t="str">
+        <v/>
+      </c>
+      <c r="H125" t="str">
+        <v/>
+      </c>
+      <c r="I125" t="str">
+        <v/>
+      </c>
+      <c r="J125" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>Selasa 07/10/2025 10:00</v>
+      </c>
+      <c r="D126" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E126" t="str">
+        <v/>
+      </c>
+      <c r="H126" t="str">
+        <v/>
+      </c>
+      <c r="I126" t="str">
+        <v/>
+      </c>
+      <c r="J126" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>Selasa 07/10/2025 11:00</v>
+      </c>
+      <c r="D127" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E127" t="str">
+        <v/>
+      </c>
+      <c r="H127" t="str">
+        <v/>
+      </c>
+      <c r="I127" t="str">
+        <v/>
+      </c>
+      <c r="J127" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>Selasa 07/10/2025 12:00</v>
+      </c>
+      <c r="D128" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E128" t="str">
+        <v/>
+      </c>
+      <c r="H128" t="str">
+        <v/>
+      </c>
+      <c r="I128" t="str">
+        <v/>
+      </c>
+      <c r="J128" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>Selasa 07/10/2025 13:00</v>
+      </c>
+      <c r="D129" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E129" t="str">
+        <v/>
+      </c>
+      <c r="H129" t="str">
+        <v/>
+      </c>
+      <c r="I129" t="str">
+        <v/>
+      </c>
+      <c r="J129" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>Selasa 07/10/2025 14:00</v>
+      </c>
+      <c r="B130">
+        <v>31</v>
+      </c>
+      <c r="C130">
+        <v>64</v>
+      </c>
+      <c r="D130" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E130" t="str">
+        <v>E (122°)</v>
+      </c>
+      <c r="F130">
+        <v>8.8</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130" t="str">
+        <v/>
+      </c>
+      <c r="I130" t="str">
+        <v/>
+      </c>
+      <c r="J130" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>Selasa 07/10/2025 15:00</v>
+      </c>
+      <c r="D131" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E131" t="str">
+        <v/>
+      </c>
+      <c r="H131" t="str">
+        <v/>
+      </c>
+      <c r="I131" t="str">
+        <v/>
+      </c>
+      <c r="J131" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>Selasa 07/10/2025 16:00</v>
+      </c>
+      <c r="D132" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E132" t="str">
+        <v/>
+      </c>
+      <c r="H132" t="str">
+        <v/>
+      </c>
+      <c r="I132" t="str">
+        <v/>
+      </c>
+      <c r="J132" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>Selasa 07/10/2025 17:00</v>
+      </c>
+      <c r="D133" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E133" t="str">
+        <v/>
+      </c>
+      <c r="H133" t="str">
+        <v/>
+      </c>
+      <c r="I133" t="str">
+        <v/>
+      </c>
+      <c r="J133" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>Selasa 07/10/2025 18:00</v>
+      </c>
+      <c r="D134" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E134" t="str">
+        <v/>
+      </c>
+      <c r="H134" t="str">
+        <v/>
+      </c>
+      <c r="I134" t="str">
+        <v/>
+      </c>
+      <c r="J134" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>Rabu 08/10/2025 07:00</v>
+      </c>
+      <c r="D135" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E135" t="str">
+        <v/>
+      </c>
+      <c r="H135" t="str">
+        <v/>
+      </c>
+      <c r="I135" t="str">
+        <v/>
+      </c>
+      <c r="J135" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>Rabu 08/10/2025 08:00</v>
+      </c>
+      <c r="B136">
+        <v>27</v>
+      </c>
+      <c r="C136">
+        <v>85</v>
+      </c>
+      <c r="D136" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E136" t="str">
+        <v>NE (87°)</v>
+      </c>
+      <c r="F136">
+        <v>4.9</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+      <c r="H136" t="str">
+        <v/>
+      </c>
+      <c r="I136" t="str">
+        <v/>
+      </c>
+      <c r="J136" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>Rabu 08/10/2025 09:00</v>
+      </c>
+      <c r="D137" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E137" t="str">
+        <v/>
+      </c>
+      <c r="H137" t="str">
+        <v/>
+      </c>
+      <c r="I137" t="str">
+        <v/>
+      </c>
+      <c r="J137" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>Rabu 08/10/2025 10:00</v>
+      </c>
+      <c r="D138" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E138" t="str">
+        <v/>
+      </c>
+      <c r="H138" t="str">
+        <v/>
+      </c>
+      <c r="I138" t="str">
+        <v/>
+      </c>
+      <c r="J138" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>Rabu 08/10/2025 11:00</v>
+      </c>
+      <c r="D139" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E139" t="str">
+        <v/>
+      </c>
+      <c r="H139" t="str">
+        <v/>
+      </c>
+      <c r="I139" t="str">
+        <v/>
+      </c>
+      <c r="J139" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>Rabu 08/10/2025 12:00</v>
+      </c>
+      <c r="D140" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E140" t="str">
+        <v/>
+      </c>
+      <c r="H140" t="str">
+        <v/>
+      </c>
+      <c r="I140" t="str">
+        <v/>
+      </c>
+      <c r="J140" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>Rabu 08/10/2025 13:00</v>
+      </c>
+      <c r="D141" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E141" t="str">
+        <v/>
+      </c>
+      <c r="H141" t="str">
+        <v/>
+      </c>
+      <c r="I141" t="str">
+        <v/>
+      </c>
+      <c r="J141" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>Rabu 08/10/2025 14:00</v>
+      </c>
+      <c r="B142">
+        <v>31</v>
+      </c>
+      <c r="C142">
+        <v>59</v>
+      </c>
+      <c r="D142" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E142" t="str">
+        <v>E (131°)</v>
+      </c>
+      <c r="F142">
+        <v>9.3</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142" t="str">
+        <v/>
+      </c>
+      <c r="I142" t="str">
+        <v/>
+      </c>
+      <c r="J142" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>Rabu 08/10/2025 15:00</v>
+      </c>
+      <c r="D143" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E143" t="str">
+        <v/>
+      </c>
+      <c r="H143" t="str">
+        <v/>
+      </c>
+      <c r="I143" t="str">
+        <v/>
+      </c>
+      <c r="J143" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>Rabu 08/10/2025 16:00</v>
+      </c>
+      <c r="D144" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E144" t="str">
+        <v/>
+      </c>
+      <c r="H144" t="str">
+        <v/>
+      </c>
+      <c r="I144" t="str">
+        <v/>
+      </c>
+      <c r="J144" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>Rabu 08/10/2025 17:00</v>
+      </c>
+      <c r="D145" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E145" t="str">
+        <v/>
+      </c>
+      <c r="H145" t="str">
+        <v/>
+      </c>
+      <c r="I145" t="str">
+        <v/>
+      </c>
+      <c r="J145" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>Rabu 08/10/2025 18:00</v>
+      </c>
+      <c r="D146" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E146" t="str">
+        <v/>
+      </c>
+      <c r="H146" t="str">
+        <v/>
+      </c>
+      <c r="I146" t="str">
+        <v/>
+      </c>
+      <c r="J146" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>Kamis 09/10/2025 07:00</v>
+      </c>
+      <c r="D147" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E147" t="str">
+        <v/>
+      </c>
+      <c r="H147" t="str">
+        <v/>
+      </c>
+      <c r="I147" t="str">
+        <v/>
+      </c>
+      <c r="J147" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>Kamis 09/10/2025 08:00</v>
+      </c>
+      <c r="B148">
+        <v>28</v>
+      </c>
+      <c r="C148">
+        <v>81</v>
+      </c>
+      <c r="D148" t="str">
+        <v>Cerah Berawan</v>
+      </c>
+      <c r="E148" t="str">
+        <v>E (123°)</v>
+      </c>
+      <c r="F148">
+        <v>8.8</v>
+      </c>
+      <c r="G148">
+        <v>0.2</v>
+      </c>
+      <c r="H148" t="str">
+        <v/>
+      </c>
+      <c r="I148" t="str">
+        <v/>
+      </c>
+      <c r="J148" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>Kamis 09/10/2025 09:00</v>
+      </c>
+      <c r="D149" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E149" t="str">
+        <v/>
+      </c>
+      <c r="H149" t="str">
+        <v/>
+      </c>
+      <c r="I149" t="str">
+        <v/>
+      </c>
+      <c r="J149" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>Kamis 09/10/2025 10:00</v>
+      </c>
+      <c r="D150" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E150" t="str">
+        <v/>
+      </c>
+      <c r="H150" t="str">
+        <v/>
+      </c>
+      <c r="I150" t="str">
+        <v/>
+      </c>
+      <c r="J150" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>Kamis 09/10/2025 11:00</v>
+      </c>
+      <c r="D151" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E151" t="str">
+        <v/>
+      </c>
+      <c r="H151" t="str">
+        <v/>
+      </c>
+      <c r="I151" t="str">
+        <v/>
+      </c>
+      <c r="J151" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>Kamis 09/10/2025 12:00</v>
+      </c>
+      <c r="D152" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E152" t="str">
+        <v/>
+      </c>
+      <c r="H152" t="str">
+        <v/>
+      </c>
+      <c r="I152" t="str">
+        <v/>
+      </c>
+      <c r="J152" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>Kamis 09/10/2025 13:00</v>
+      </c>
+      <c r="D153" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E153" t="str">
+        <v/>
+      </c>
+      <c r="H153" t="str">
+        <v/>
+      </c>
+      <c r="I153" t="str">
+        <v/>
+      </c>
+      <c r="J153" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>Kamis 09/10/2025 14:00</v>
+      </c>
+      <c r="D154" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E154" t="str">
+        <v/>
+      </c>
+      <c r="H154" t="str">
+        <v/>
+      </c>
+      <c r="I154" t="str">
+        <v/>
+      </c>
+      <c r="J154" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>Kamis 09/10/2025 15:00</v>
+      </c>
+      <c r="D155" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E155" t="str">
+        <v/>
+      </c>
+      <c r="H155" t="str">
+        <v/>
+      </c>
+      <c r="I155" t="str">
+        <v/>
+      </c>
+      <c r="J155" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>Kamis 09/10/2025 16:00</v>
+      </c>
+      <c r="D156" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E156" t="str">
+        <v/>
+      </c>
+      <c r="H156" t="str">
+        <v/>
+      </c>
+      <c r="I156" t="str">
+        <v/>
+      </c>
+      <c r="J156" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>Kamis 09/10/2025 17:00</v>
+      </c>
+      <c r="D157" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E157" t="str">
+        <v/>
+      </c>
+      <c r="H157" t="str">
+        <v/>
+      </c>
+      <c r="I157" t="str">
+        <v/>
+      </c>
+      <c r="J157" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>Kamis 09/10/2025 18:00</v>
+      </c>
+      <c r="D158" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E158" t="str">
+        <v/>
+      </c>
+      <c r="H158" t="str">
+        <v/>
+      </c>
+      <c r="I158" t="str">
+        <v/>
+      </c>
+      <c r="J158" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J158"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
save all from replit
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2205,10 +2205,10 @@
         <v>Selasa 30/09/2025 11:00</v>
       </c>
       <c r="B79">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C79">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D79" t="str">
         <v>Hujan Ringan</v>
@@ -2220,7 +2220,7 @@
         <v>5.2</v>
       </c>
       <c r="G79">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
       <c r="H79" t="str">
         <v/>
@@ -2237,22 +2237,22 @@
         <v>Selasa 30/09/2025 12:00</v>
       </c>
       <c r="B80">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C80">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D80" t="str">
-        <v>Hujan Petir</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E80" t="str">
-        <v>SW (262°)</v>
+        <v>E (114°)</v>
       </c>
       <c r="F80">
-        <v>7.4</v>
+        <v>8</v>
       </c>
       <c r="G80">
-        <v>3.8</v>
+        <v>2.7</v>
       </c>
       <c r="H80" t="str">
         <v/>
@@ -2269,13 +2269,13 @@
         <v>Selasa 30/09/2025 13:00</v>
       </c>
       <c r="B81">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C81">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D81" t="str">
-        <v>Hujan Petir</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E81" t="str">
         <v>E (114°)</v>
@@ -2284,7 +2284,7 @@
         <v>8</v>
       </c>
       <c r="G81">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
       <c r="H81" t="str">
         <v/>
@@ -2301,13 +2301,13 @@
         <v>Selasa 30/09/2025 14:00</v>
       </c>
       <c r="B82">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C82">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D82" t="str">
-        <v>Hujan Petir</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E82" t="str">
         <v>E (114°)</v>
@@ -2316,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="G82">
-        <v>3.7</v>
+        <v>2.7</v>
       </c>
       <c r="H82" t="str">
         <v/>
@@ -2336,19 +2336,19 @@
         <v>26</v>
       </c>
       <c r="C83">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D83" t="str">
-        <v>Berawan</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E83" t="str">
-        <v>NE (53°)</v>
+        <v>NE (62°)</v>
       </c>
       <c r="F83">
-        <v>3.6</v>
+        <v>5.3</v>
       </c>
       <c r="G83">
-        <v>0.8</v>
+        <v>2.7</v>
       </c>
       <c r="H83" t="str">
         <v/>
@@ -2365,13 +2365,13 @@
         <v>Selasa 30/09/2025 16:00</v>
       </c>
       <c r="B84">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C84">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D84" t="str">
-        <v>Hujan Petir</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E84" t="str">
         <v>NE (62°)</v>
@@ -2380,7 +2380,7 @@
         <v>5.3</v>
       </c>
       <c r="G84">
-        <v>3.7</v>
+        <v>2.7</v>
       </c>
       <c r="H84" t="str">
         <v/>
@@ -2397,13 +2397,13 @@
         <v>Selasa 30/09/2025 17:00</v>
       </c>
       <c r="B85">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C85">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D85" t="str">
-        <v>Petir</v>
+        <v>Berawan</v>
       </c>
       <c r="E85" t="str">
         <v>NE (62°)</v>
@@ -2429,19 +2429,19 @@
         <v>Selasa 30/09/2025 18:00</v>
       </c>
       <c r="B86">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C86">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D86" t="str">
-        <v>Cerah Berawan</v>
+        <v>Berawan</v>
       </c>
       <c r="E86" t="str">
-        <v>NE (45°)</v>
+        <v>N (14°)</v>
       </c>
       <c r="F86">
-        <v>4.7</v>
+        <v>4.2</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -2464,19 +2464,19 @@
         <v>24</v>
       </c>
       <c r="C87">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D87" t="str">
-        <v>Hujan Ringan</v>
+        <v>Cerah</v>
       </c>
       <c r="E87" t="str">
-        <v>S (224°)</v>
+        <v>N (10°)</v>
       </c>
       <c r="F87">
-        <v>6.9</v>
+        <v>7.5</v>
       </c>
       <c r="G87">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="H87" t="str">
         <v/>
@@ -2493,22 +2493,22 @@
         <v>Rabu 01/10/2025 08:00</v>
       </c>
       <c r="B88">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C88">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D88" t="str">
-        <v>Cerah</v>
+        <v>Berawan</v>
       </c>
       <c r="E88" t="str">
-        <v>S (224°)</v>
+        <v>N (10°)</v>
       </c>
       <c r="F88">
-        <v>6.9</v>
+        <v>7.5</v>
       </c>
       <c r="G88">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H88" t="str">
         <v/>
@@ -2589,22 +2589,22 @@
         <v>Rabu 01/10/2025 11:00</v>
       </c>
       <c r="B91">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C91">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D91" t="str">
         <v>Cerah</v>
       </c>
       <c r="E91" t="str">
-        <v>E (107°)</v>
+        <v>NE (70°)</v>
       </c>
       <c r="F91">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91" t="str">
         <v/>
@@ -2685,22 +2685,22 @@
         <v>Rabu 01/10/2025 14:00</v>
       </c>
       <c r="B94">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C94">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D94" t="str">
-        <v>Cerah</v>
+        <v>Hujan Ringan</v>
       </c>
       <c r="E94" t="str">
-        <v>E (129°)</v>
+        <v>SE (160°)</v>
       </c>
       <c r="F94">
-        <v>14.1</v>
+        <v>18.5</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="H94" t="str">
         <v/>
@@ -2781,19 +2781,19 @@
         <v>Rabu 01/10/2025 17:00</v>
       </c>
       <c r="B97">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C97">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D97" t="str">
         <v>Cerah</v>
       </c>
       <c r="E97" t="str">
-        <v>E (127°)</v>
+        <v>S (200°)</v>
       </c>
       <c r="F97">
-        <v>13.3</v>
+        <v>18.5</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -2877,19 +2877,19 @@
         <v>Kamis 02/10/2025 08:00</v>
       </c>
       <c r="B100">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C100">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D100" t="str">
         <v>Cerah</v>
       </c>
       <c r="E100" t="str">
-        <v>NE (65°)</v>
+        <v>N (20°)</v>
       </c>
       <c r="F100">
-        <v>7.9</v>
+        <v>8.3</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -2949,10 +2949,10 @@
         <v>Kamis 02/10/2025 11:00</v>
       </c>
       <c r="B103">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C103">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D103" t="str">
         <v>Cerah</v>
@@ -3096,13 +3096,13 @@
         <v>28</v>
       </c>
       <c r="C109">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D109" t="str">
         <v>Cerah</v>
       </c>
       <c r="E109" t="str">
-        <v>E (126°)</v>
+        <v>E (127°)</v>
       </c>
       <c r="F109">
         <v>10.8</v>
@@ -3137,6 +3137,1866 @@
         <v/>
       </c>
       <c r="J110" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>Jumat 03/10/2025 07:00</v>
+      </c>
+      <c r="D111" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E111" t="str">
+        <v/>
+      </c>
+      <c r="H111" t="str">
+        <v/>
+      </c>
+      <c r="I111" t="str">
+        <v/>
+      </c>
+      <c r="J111" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>Jumat 03/10/2025 08:00</v>
+      </c>
+      <c r="B112">
+        <v>29</v>
+      </c>
+      <c r="C112">
+        <v>71</v>
+      </c>
+      <c r="D112" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E112" t="str">
+        <v>E (103°)</v>
+      </c>
+      <c r="F112">
+        <v>5.9</v>
+      </c>
+      <c r="G112">
+        <v>0.2</v>
+      </c>
+      <c r="H112" t="str">
+        <v/>
+      </c>
+      <c r="I112" t="str">
+        <v/>
+      </c>
+      <c r="J112" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>Jumat 03/10/2025 09:00</v>
+      </c>
+      <c r="D113" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E113" t="str">
+        <v/>
+      </c>
+      <c r="H113" t="str">
+        <v/>
+      </c>
+      <c r="I113" t="str">
+        <v/>
+      </c>
+      <c r="J113" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>Jumat 03/10/2025 10:00</v>
+      </c>
+      <c r="D114" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E114" t="str">
+        <v/>
+      </c>
+      <c r="H114" t="str">
+        <v/>
+      </c>
+      <c r="I114" t="str">
+        <v/>
+      </c>
+      <c r="J114" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>Jumat 03/10/2025 11:00</v>
+      </c>
+      <c r="B115">
+        <v>31</v>
+      </c>
+      <c r="C115">
+        <v>64</v>
+      </c>
+      <c r="D115" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E115" t="str">
+        <v>E (131°)</v>
+      </c>
+      <c r="F115">
+        <v>12.3</v>
+      </c>
+      <c r="G115">
+        <v>0.2</v>
+      </c>
+      <c r="H115" t="str">
+        <v/>
+      </c>
+      <c r="I115" t="str">
+        <v/>
+      </c>
+      <c r="J115" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>Jumat 03/10/2025 12:00</v>
+      </c>
+      <c r="D116" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E116" t="str">
+        <v/>
+      </c>
+      <c r="H116" t="str">
+        <v/>
+      </c>
+      <c r="I116" t="str">
+        <v/>
+      </c>
+      <c r="J116" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>Jumat 03/10/2025 13:00</v>
+      </c>
+      <c r="D117" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E117" t="str">
+        <v/>
+      </c>
+      <c r="H117" t="str">
+        <v/>
+      </c>
+      <c r="I117" t="str">
+        <v/>
+      </c>
+      <c r="J117" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>Jumat 03/10/2025 14:00</v>
+      </c>
+      <c r="B118">
+        <v>30</v>
+      </c>
+      <c r="C118">
+        <v>64</v>
+      </c>
+      <c r="D118" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E118" t="str">
+        <v>E (131°)</v>
+      </c>
+      <c r="F118">
+        <v>12.3</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118" t="str">
+        <v/>
+      </c>
+      <c r="I118" t="str">
+        <v/>
+      </c>
+      <c r="J118" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>Jumat 03/10/2025 15:00</v>
+      </c>
+      <c r="D119" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E119" t="str">
+        <v/>
+      </c>
+      <c r="H119" t="str">
+        <v/>
+      </c>
+      <c r="I119" t="str">
+        <v/>
+      </c>
+      <c r="J119" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>Jumat 03/10/2025 16:00</v>
+      </c>
+      <c r="D120" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E120" t="str">
+        <v/>
+      </c>
+      <c r="H120" t="str">
+        <v/>
+      </c>
+      <c r="I120" t="str">
+        <v/>
+      </c>
+      <c r="J120" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>Jumat 03/10/2025 17:00</v>
+      </c>
+      <c r="B121">
+        <v>29</v>
+      </c>
+      <c r="C121">
+        <v>69</v>
+      </c>
+      <c r="D121" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E121" t="str">
+        <v>NE (86°)</v>
+      </c>
+      <c r="F121">
+        <v>14</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121" t="str">
+        <v/>
+      </c>
+      <c r="I121" t="str">
+        <v/>
+      </c>
+      <c r="J121" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>Jumat 03/10/2025 18:00</v>
+      </c>
+      <c r="D122" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E122" t="str">
+        <v/>
+      </c>
+      <c r="H122" t="str">
+        <v/>
+      </c>
+      <c r="I122" t="str">
+        <v/>
+      </c>
+      <c r="J122" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>Sabtu 04/10/2025 07:00</v>
+      </c>
+      <c r="D123" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E123" t="str">
+        <v/>
+      </c>
+      <c r="H123" t="str">
+        <v/>
+      </c>
+      <c r="I123" t="str">
+        <v/>
+      </c>
+      <c r="J123" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>Sabtu 04/10/2025 08:00</v>
+      </c>
+      <c r="B124">
+        <v>27</v>
+      </c>
+      <c r="C124">
+        <v>83</v>
+      </c>
+      <c r="D124" t="str">
+        <v>Cerah Berawan</v>
+      </c>
+      <c r="E124" t="str">
+        <v>NE (81°)</v>
+      </c>
+      <c r="F124">
+        <v>15</v>
+      </c>
+      <c r="G124">
+        <v>0.2</v>
+      </c>
+      <c r="H124" t="str">
+        <v/>
+      </c>
+      <c r="I124" t="str">
+        <v/>
+      </c>
+      <c r="J124" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>Sabtu 04/10/2025 09:00</v>
+      </c>
+      <c r="D125" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E125" t="str">
+        <v/>
+      </c>
+      <c r="H125" t="str">
+        <v/>
+      </c>
+      <c r="I125" t="str">
+        <v/>
+      </c>
+      <c r="J125" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>Sabtu 04/10/2025 10:00</v>
+      </c>
+      <c r="D126" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E126" t="str">
+        <v/>
+      </c>
+      <c r="H126" t="str">
+        <v/>
+      </c>
+      <c r="I126" t="str">
+        <v/>
+      </c>
+      <c r="J126" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>Sabtu 04/10/2025 11:00</v>
+      </c>
+      <c r="D127" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E127" t="str">
+        <v/>
+      </c>
+      <c r="H127" t="str">
+        <v/>
+      </c>
+      <c r="I127" t="str">
+        <v/>
+      </c>
+      <c r="J127" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>Sabtu 04/10/2025 12:00</v>
+      </c>
+      <c r="D128" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E128" t="str">
+        <v/>
+      </c>
+      <c r="H128" t="str">
+        <v/>
+      </c>
+      <c r="I128" t="str">
+        <v/>
+      </c>
+      <c r="J128" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>Sabtu 04/10/2025 13:00</v>
+      </c>
+      <c r="D129" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E129" t="str">
+        <v/>
+      </c>
+      <c r="H129" t="str">
+        <v/>
+      </c>
+      <c r="I129" t="str">
+        <v/>
+      </c>
+      <c r="J129" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>Sabtu 04/10/2025 14:00</v>
+      </c>
+      <c r="B130">
+        <v>29</v>
+      </c>
+      <c r="C130">
+        <v>72</v>
+      </c>
+      <c r="D130" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E130" t="str">
+        <v>E (104°)</v>
+      </c>
+      <c r="F130">
+        <v>7.2</v>
+      </c>
+      <c r="G130">
+        <v>0.2</v>
+      </c>
+      <c r="H130" t="str">
+        <v/>
+      </c>
+      <c r="I130" t="str">
+        <v/>
+      </c>
+      <c r="J130" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>Sabtu 04/10/2025 15:00</v>
+      </c>
+      <c r="D131" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E131" t="str">
+        <v/>
+      </c>
+      <c r="H131" t="str">
+        <v/>
+      </c>
+      <c r="I131" t="str">
+        <v/>
+      </c>
+      <c r="J131" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>Sabtu 04/10/2025 16:00</v>
+      </c>
+      <c r="D132" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E132" t="str">
+        <v/>
+      </c>
+      <c r="H132" t="str">
+        <v/>
+      </c>
+      <c r="I132" t="str">
+        <v/>
+      </c>
+      <c r="J132" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>Sabtu 04/10/2025 17:00</v>
+      </c>
+      <c r="D133" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E133" t="str">
+        <v/>
+      </c>
+      <c r="H133" t="str">
+        <v/>
+      </c>
+      <c r="I133" t="str">
+        <v/>
+      </c>
+      <c r="J133" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>Sabtu 04/10/2025 18:00</v>
+      </c>
+      <c r="D134" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E134" t="str">
+        <v/>
+      </c>
+      <c r="H134" t="str">
+        <v/>
+      </c>
+      <c r="I134" t="str">
+        <v/>
+      </c>
+      <c r="J134" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>Minggu 05/10/2025 07:00</v>
+      </c>
+      <c r="D135" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E135" t="str">
+        <v/>
+      </c>
+      <c r="H135" t="str">
+        <v/>
+      </c>
+      <c r="I135" t="str">
+        <v/>
+      </c>
+      <c r="J135" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>Minggu 05/10/2025 08:00</v>
+      </c>
+      <c r="B136">
+        <v>24</v>
+      </c>
+      <c r="C136">
+        <v>95</v>
+      </c>
+      <c r="D136" t="str">
+        <v>Petir</v>
+      </c>
+      <c r="E136" t="str">
+        <v>N (10°)</v>
+      </c>
+      <c r="F136">
+        <v>1.1</v>
+      </c>
+      <c r="G136">
+        <v>0.3</v>
+      </c>
+      <c r="H136" t="str">
+        <v/>
+      </c>
+      <c r="I136" t="str">
+        <v/>
+      </c>
+      <c r="J136" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>Minggu 05/10/2025 09:00</v>
+      </c>
+      <c r="D137" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E137" t="str">
+        <v/>
+      </c>
+      <c r="H137" t="str">
+        <v/>
+      </c>
+      <c r="I137" t="str">
+        <v/>
+      </c>
+      <c r="J137" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>Minggu 05/10/2025 10:00</v>
+      </c>
+      <c r="D138" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E138" t="str">
+        <v/>
+      </c>
+      <c r="H138" t="str">
+        <v/>
+      </c>
+      <c r="I138" t="str">
+        <v/>
+      </c>
+      <c r="J138" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>Minggu 05/10/2025 11:00</v>
+      </c>
+      <c r="D139" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E139" t="str">
+        <v/>
+      </c>
+      <c r="H139" t="str">
+        <v/>
+      </c>
+      <c r="I139" t="str">
+        <v/>
+      </c>
+      <c r="J139" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>Minggu 05/10/2025 12:00</v>
+      </c>
+      <c r="D140" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E140" t="str">
+        <v/>
+      </c>
+      <c r="H140" t="str">
+        <v/>
+      </c>
+      <c r="I140" t="str">
+        <v/>
+      </c>
+      <c r="J140" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>Minggu 05/10/2025 13:00</v>
+      </c>
+      <c r="D141" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E141" t="str">
+        <v/>
+      </c>
+      <c r="H141" t="str">
+        <v/>
+      </c>
+      <c r="I141" t="str">
+        <v/>
+      </c>
+      <c r="J141" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>Minggu 05/10/2025 14:00</v>
+      </c>
+      <c r="B142">
+        <v>29</v>
+      </c>
+      <c r="C142">
+        <v>72</v>
+      </c>
+      <c r="D142" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E142" t="str">
+        <v>E (99°)</v>
+      </c>
+      <c r="F142">
+        <v>9.5</v>
+      </c>
+      <c r="G142">
+        <v>0.3</v>
+      </c>
+      <c r="H142" t="str">
+        <v/>
+      </c>
+      <c r="I142" t="str">
+        <v/>
+      </c>
+      <c r="J142" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>Minggu 05/10/2025 15:00</v>
+      </c>
+      <c r="D143" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E143" t="str">
+        <v/>
+      </c>
+      <c r="H143" t="str">
+        <v/>
+      </c>
+      <c r="I143" t="str">
+        <v/>
+      </c>
+      <c r="J143" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>Minggu 05/10/2025 16:00</v>
+      </c>
+      <c r="D144" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E144" t="str">
+        <v/>
+      </c>
+      <c r="H144" t="str">
+        <v/>
+      </c>
+      <c r="I144" t="str">
+        <v/>
+      </c>
+      <c r="J144" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>Minggu 05/10/2025 17:00</v>
+      </c>
+      <c r="D145" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E145" t="str">
+        <v/>
+      </c>
+      <c r="H145" t="str">
+        <v/>
+      </c>
+      <c r="I145" t="str">
+        <v/>
+      </c>
+      <c r="J145" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>Minggu 05/10/2025 18:00</v>
+      </c>
+      <c r="D146" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E146" t="str">
+        <v/>
+      </c>
+      <c r="H146" t="str">
+        <v/>
+      </c>
+      <c r="I146" t="str">
+        <v/>
+      </c>
+      <c r="J146" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>Senin 06/10/2025 07:00</v>
+      </c>
+      <c r="D147" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E147" t="str">
+        <v/>
+      </c>
+      <c r="H147" t="str">
+        <v/>
+      </c>
+      <c r="I147" t="str">
+        <v/>
+      </c>
+      <c r="J147" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>Senin 06/10/2025 08:00</v>
+      </c>
+      <c r="B148">
+        <v>23</v>
+      </c>
+      <c r="C148">
+        <v>95</v>
+      </c>
+      <c r="D148" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E148" t="str">
+        <v>SW (246°)</v>
+      </c>
+      <c r="F148">
+        <v>2.6</v>
+      </c>
+      <c r="G148">
+        <v>0.1</v>
+      </c>
+      <c r="H148" t="str">
+        <v/>
+      </c>
+      <c r="I148" t="str">
+        <v/>
+      </c>
+      <c r="J148" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>Senin 06/10/2025 09:00</v>
+      </c>
+      <c r="D149" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E149" t="str">
+        <v/>
+      </c>
+      <c r="H149" t="str">
+        <v/>
+      </c>
+      <c r="I149" t="str">
+        <v/>
+      </c>
+      <c r="J149" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>Senin 06/10/2025 10:00</v>
+      </c>
+      <c r="D150" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E150" t="str">
+        <v/>
+      </c>
+      <c r="H150" t="str">
+        <v/>
+      </c>
+      <c r="I150" t="str">
+        <v/>
+      </c>
+      <c r="J150" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>Senin 06/10/2025 11:00</v>
+      </c>
+      <c r="D151" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E151" t="str">
+        <v/>
+      </c>
+      <c r="H151" t="str">
+        <v/>
+      </c>
+      <c r="I151" t="str">
+        <v/>
+      </c>
+      <c r="J151" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>Senin 06/10/2025 12:00</v>
+      </c>
+      <c r="D152" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E152" t="str">
+        <v/>
+      </c>
+      <c r="H152" t="str">
+        <v/>
+      </c>
+      <c r="I152" t="str">
+        <v/>
+      </c>
+      <c r="J152" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>Senin 06/10/2025 13:00</v>
+      </c>
+      <c r="D153" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E153" t="str">
+        <v/>
+      </c>
+      <c r="H153" t="str">
+        <v/>
+      </c>
+      <c r="I153" t="str">
+        <v/>
+      </c>
+      <c r="J153" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>Senin 06/10/2025 14:00</v>
+      </c>
+      <c r="B154">
+        <v>30</v>
+      </c>
+      <c r="C154">
+        <v>70</v>
+      </c>
+      <c r="D154" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E154" t="str">
+        <v>E (90°)</v>
+      </c>
+      <c r="F154">
+        <v>9.6</v>
+      </c>
+      <c r="G154">
+        <v>0.1</v>
+      </c>
+      <c r="H154" t="str">
+        <v/>
+      </c>
+      <c r="I154" t="str">
+        <v/>
+      </c>
+      <c r="J154" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>Senin 06/10/2025 15:00</v>
+      </c>
+      <c r="D155" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E155" t="str">
+        <v/>
+      </c>
+      <c r="H155" t="str">
+        <v/>
+      </c>
+      <c r="I155" t="str">
+        <v/>
+      </c>
+      <c r="J155" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>Senin 06/10/2025 16:00</v>
+      </c>
+      <c r="D156" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E156" t="str">
+        <v/>
+      </c>
+      <c r="H156" t="str">
+        <v/>
+      </c>
+      <c r="I156" t="str">
+        <v/>
+      </c>
+      <c r="J156" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>Senin 06/10/2025 17:00</v>
+      </c>
+      <c r="D157" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E157" t="str">
+        <v/>
+      </c>
+      <c r="H157" t="str">
+        <v/>
+      </c>
+      <c r="I157" t="str">
+        <v/>
+      </c>
+      <c r="J157" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>Senin 06/10/2025 18:00</v>
+      </c>
+      <c r="D158" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E158" t="str">
+        <v/>
+      </c>
+      <c r="H158" t="str">
+        <v/>
+      </c>
+      <c r="I158" t="str">
+        <v/>
+      </c>
+      <c r="J158" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>Selasa 07/10/2025 07:00</v>
+      </c>
+      <c r="D159" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E159" t="str">
+        <v/>
+      </c>
+      <c r="H159" t="str">
+        <v/>
+      </c>
+      <c r="I159" t="str">
+        <v/>
+      </c>
+      <c r="J159" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>Selasa 07/10/2025 08:00</v>
+      </c>
+      <c r="B160">
+        <v>26</v>
+      </c>
+      <c r="C160">
+        <v>87</v>
+      </c>
+      <c r="D160" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E160" t="str">
+        <v>NE (83°)</v>
+      </c>
+      <c r="F160">
+        <v>6.9</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160" t="str">
+        <v/>
+      </c>
+      <c r="I160" t="str">
+        <v/>
+      </c>
+      <c r="J160" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>Selasa 07/10/2025 09:00</v>
+      </c>
+      <c r="D161" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E161" t="str">
+        <v/>
+      </c>
+      <c r="H161" t="str">
+        <v/>
+      </c>
+      <c r="I161" t="str">
+        <v/>
+      </c>
+      <c r="J161" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>Selasa 07/10/2025 10:00</v>
+      </c>
+      <c r="D162" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E162" t="str">
+        <v/>
+      </c>
+      <c r="H162" t="str">
+        <v/>
+      </c>
+      <c r="I162" t="str">
+        <v/>
+      </c>
+      <c r="J162" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>Selasa 07/10/2025 11:00</v>
+      </c>
+      <c r="D163" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E163" t="str">
+        <v/>
+      </c>
+      <c r="H163" t="str">
+        <v/>
+      </c>
+      <c r="I163" t="str">
+        <v/>
+      </c>
+      <c r="J163" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>Selasa 07/10/2025 12:00</v>
+      </c>
+      <c r="D164" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E164" t="str">
+        <v/>
+      </c>
+      <c r="H164" t="str">
+        <v/>
+      </c>
+      <c r="I164" t="str">
+        <v/>
+      </c>
+      <c r="J164" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>Selasa 07/10/2025 13:00</v>
+      </c>
+      <c r="D165" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E165" t="str">
+        <v/>
+      </c>
+      <c r="H165" t="str">
+        <v/>
+      </c>
+      <c r="I165" t="str">
+        <v/>
+      </c>
+      <c r="J165" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>Selasa 07/10/2025 14:00</v>
+      </c>
+      <c r="B166">
+        <v>31</v>
+      </c>
+      <c r="C166">
+        <v>64</v>
+      </c>
+      <c r="D166" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E166" t="str">
+        <v>E (122°)</v>
+      </c>
+      <c r="F166">
+        <v>8.8</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166" t="str">
+        <v/>
+      </c>
+      <c r="I166" t="str">
+        <v/>
+      </c>
+      <c r="J166" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>Selasa 07/10/2025 15:00</v>
+      </c>
+      <c r="D167" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E167" t="str">
+        <v/>
+      </c>
+      <c r="H167" t="str">
+        <v/>
+      </c>
+      <c r="I167" t="str">
+        <v/>
+      </c>
+      <c r="J167" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>Selasa 07/10/2025 16:00</v>
+      </c>
+      <c r="D168" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E168" t="str">
+        <v/>
+      </c>
+      <c r="H168" t="str">
+        <v/>
+      </c>
+      <c r="I168" t="str">
+        <v/>
+      </c>
+      <c r="J168" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>Selasa 07/10/2025 17:00</v>
+      </c>
+      <c r="D169" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E169" t="str">
+        <v/>
+      </c>
+      <c r="H169" t="str">
+        <v/>
+      </c>
+      <c r="I169" t="str">
+        <v/>
+      </c>
+      <c r="J169" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>Selasa 07/10/2025 18:00</v>
+      </c>
+      <c r="D170" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E170" t="str">
+        <v/>
+      </c>
+      <c r="H170" t="str">
+        <v/>
+      </c>
+      <c r="I170" t="str">
+        <v/>
+      </c>
+      <c r="J170" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>Rabu 08/10/2025 07:00</v>
+      </c>
+      <c r="D171" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E171" t="str">
+        <v/>
+      </c>
+      <c r="H171" t="str">
+        <v/>
+      </c>
+      <c r="I171" t="str">
+        <v/>
+      </c>
+      <c r="J171" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>Rabu 08/10/2025 08:00</v>
+      </c>
+      <c r="B172">
+        <v>27</v>
+      </c>
+      <c r="C172">
+        <v>85</v>
+      </c>
+      <c r="D172" t="str">
+        <v>Berawan</v>
+      </c>
+      <c r="E172" t="str">
+        <v>NE (87°)</v>
+      </c>
+      <c r="F172">
+        <v>4.9</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172" t="str">
+        <v/>
+      </c>
+      <c r="I172" t="str">
+        <v/>
+      </c>
+      <c r="J172" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>Rabu 08/10/2025 09:00</v>
+      </c>
+      <c r="D173" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E173" t="str">
+        <v/>
+      </c>
+      <c r="H173" t="str">
+        <v/>
+      </c>
+      <c r="I173" t="str">
+        <v/>
+      </c>
+      <c r="J173" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>Rabu 08/10/2025 10:00</v>
+      </c>
+      <c r="D174" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E174" t="str">
+        <v/>
+      </c>
+      <c r="H174" t="str">
+        <v/>
+      </c>
+      <c r="I174" t="str">
+        <v/>
+      </c>
+      <c r="J174" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>Rabu 08/10/2025 11:00</v>
+      </c>
+      <c r="D175" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E175" t="str">
+        <v/>
+      </c>
+      <c r="H175" t="str">
+        <v/>
+      </c>
+      <c r="I175" t="str">
+        <v/>
+      </c>
+      <c r="J175" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>Rabu 08/10/2025 12:00</v>
+      </c>
+      <c r="D176" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E176" t="str">
+        <v/>
+      </c>
+      <c r="H176" t="str">
+        <v/>
+      </c>
+      <c r="I176" t="str">
+        <v/>
+      </c>
+      <c r="J176" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>Rabu 08/10/2025 13:00</v>
+      </c>
+      <c r="D177" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E177" t="str">
+        <v/>
+      </c>
+      <c r="H177" t="str">
+        <v/>
+      </c>
+      <c r="I177" t="str">
+        <v/>
+      </c>
+      <c r="J177" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>Rabu 08/10/2025 14:00</v>
+      </c>
+      <c r="B178">
+        <v>31</v>
+      </c>
+      <c r="C178">
+        <v>59</v>
+      </c>
+      <c r="D178" t="str">
+        <v>Cerah</v>
+      </c>
+      <c r="E178" t="str">
+        <v>E (131°)</v>
+      </c>
+      <c r="F178">
+        <v>9.3</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178" t="str">
+        <v/>
+      </c>
+      <c r="I178" t="str">
+        <v/>
+      </c>
+      <c r="J178" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>Rabu 08/10/2025 15:00</v>
+      </c>
+      <c r="D179" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E179" t="str">
+        <v/>
+      </c>
+      <c r="H179" t="str">
+        <v/>
+      </c>
+      <c r="I179" t="str">
+        <v/>
+      </c>
+      <c r="J179" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>Rabu 08/10/2025 16:00</v>
+      </c>
+      <c r="D180" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E180" t="str">
+        <v/>
+      </c>
+      <c r="H180" t="str">
+        <v/>
+      </c>
+      <c r="I180" t="str">
+        <v/>
+      </c>
+      <c r="J180" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>Rabu 08/10/2025 17:00</v>
+      </c>
+      <c r="D181" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E181" t="str">
+        <v/>
+      </c>
+      <c r="H181" t="str">
+        <v/>
+      </c>
+      <c r="I181" t="str">
+        <v/>
+      </c>
+      <c r="J181" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>Rabu 08/10/2025 18:00</v>
+      </c>
+      <c r="D182" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E182" t="str">
+        <v/>
+      </c>
+      <c r="H182" t="str">
+        <v/>
+      </c>
+      <c r="I182" t="str">
+        <v/>
+      </c>
+      <c r="J182" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>Kamis 09/10/2025 07:00</v>
+      </c>
+      <c r="D183" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E183" t="str">
+        <v/>
+      </c>
+      <c r="H183" t="str">
+        <v/>
+      </c>
+      <c r="I183" t="str">
+        <v/>
+      </c>
+      <c r="J183" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>Kamis 09/10/2025 08:00</v>
+      </c>
+      <c r="B184">
+        <v>28</v>
+      </c>
+      <c r="C184">
+        <v>81</v>
+      </c>
+      <c r="D184" t="str">
+        <v>Cerah Berawan</v>
+      </c>
+      <c r="E184" t="str">
+        <v>E (123°)</v>
+      </c>
+      <c r="F184">
+        <v>8.8</v>
+      </c>
+      <c r="G184">
+        <v>0.2</v>
+      </c>
+      <c r="H184" t="str">
+        <v/>
+      </c>
+      <c r="I184" t="str">
+        <v/>
+      </c>
+      <c r="J184" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>Kamis 09/10/2025 09:00</v>
+      </c>
+      <c r="D185" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E185" t="str">
+        <v/>
+      </c>
+      <c r="H185" t="str">
+        <v/>
+      </c>
+      <c r="I185" t="str">
+        <v/>
+      </c>
+      <c r="J185" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>Kamis 09/10/2025 10:00</v>
+      </c>
+      <c r="D186" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E186" t="str">
+        <v/>
+      </c>
+      <c r="H186" t="str">
+        <v/>
+      </c>
+      <c r="I186" t="str">
+        <v/>
+      </c>
+      <c r="J186" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>Kamis 09/10/2025 11:00</v>
+      </c>
+      <c r="D187" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E187" t="str">
+        <v/>
+      </c>
+      <c r="H187" t="str">
+        <v/>
+      </c>
+      <c r="I187" t="str">
+        <v/>
+      </c>
+      <c r="J187" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>Kamis 09/10/2025 12:00</v>
+      </c>
+      <c r="D188" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E188" t="str">
+        <v/>
+      </c>
+      <c r="H188" t="str">
+        <v/>
+      </c>
+      <c r="I188" t="str">
+        <v/>
+      </c>
+      <c r="J188" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>Kamis 09/10/2025 13:00</v>
+      </c>
+      <c r="D189" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E189" t="str">
+        <v/>
+      </c>
+      <c r="H189" t="str">
+        <v/>
+      </c>
+      <c r="I189" t="str">
+        <v/>
+      </c>
+      <c r="J189" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>Kamis 09/10/2025 14:00</v>
+      </c>
+      <c r="D190" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E190" t="str">
+        <v/>
+      </c>
+      <c r="H190" t="str">
+        <v/>
+      </c>
+      <c r="I190" t="str">
+        <v/>
+      </c>
+      <c r="J190" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>Kamis 09/10/2025 15:00</v>
+      </c>
+      <c r="D191" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E191" t="str">
+        <v/>
+      </c>
+      <c r="H191" t="str">
+        <v/>
+      </c>
+      <c r="I191" t="str">
+        <v/>
+      </c>
+      <c r="J191" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>Kamis 09/10/2025 16:00</v>
+      </c>
+      <c r="D192" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E192" t="str">
+        <v/>
+      </c>
+      <c r="H192" t="str">
+        <v/>
+      </c>
+      <c r="I192" t="str">
+        <v/>
+      </c>
+      <c r="J192" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>Kamis 09/10/2025 17:00</v>
+      </c>
+      <c r="D193" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E193" t="str">
+        <v/>
+      </c>
+      <c r="H193" t="str">
+        <v/>
+      </c>
+      <c r="I193" t="str">
+        <v/>
+      </c>
+      <c r="J193" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>Kamis 09/10/2025 18:00</v>
+      </c>
+      <c r="D194" t="str">
+        <v>Tidak ada data</v>
+      </c>
+      <c r="E194" t="str">
+        <v/>
+      </c>
+      <c r="H194" t="str">
+        <v/>
+      </c>
+      <c r="I194" t="str">
+        <v/>
+      </c>
+      <c r="J194" t="str">
         <v/>
       </c>
     </row>
@@ -3146,7 +5006,7 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J110"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J194"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>